<commit_message>
Fixed: EntityContainer need to expose only resourcesets, not types
</commit_message>
<xml_diff>
--- a/MR3/tests/test odata stuff.xlsx
+++ b/MR3/tests/test odata stuff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="19200" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="missing" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="106">
   <si>
     <t>Missing features</t>
   </si>
@@ -334,6 +334,18 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Http Result</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>201/+Location</t>
+  </si>
+  <si>
+    <t>Op Result</t>
   </si>
 </sst>
 </file>
@@ -478,7 +490,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -490,45 +502,55 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1071,92 +1093,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I66"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="4" width="8.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="4" width="5.140625" style="9" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="43" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="43" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="19"/>
-    </row>
-    <row r="2" spans="2:9" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="12"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="2:9" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
-      <c r="B3" s="16" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="12"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="2:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="16"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" s="6" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-    </row>
-    <row r="6" spans="2:9" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="G5" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="15" t="s">
+      <c r="G6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="J6" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
         <v>101</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1168,11 +1218,14 @@
       <c r="G7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="16">
+        <v>200</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1182,11 +1235,14 @@
       <c r="G8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="16">
+        <v>200</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1196,11 +1252,14 @@
       <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="16">
+        <v>200</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10" s="4" t="s">
         <v>19</v>
       </c>
@@ -1210,11 +1269,14 @@
       <c r="G10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="16">
+        <v>200</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1224,11 +1286,14 @@
       <c r="G11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="16">
+        <v>200</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E12" s="4" t="s">
         <v>19</v>
       </c>
@@ -1238,12 +1303,15 @@
       <c r="G12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="16">
+        <v>200</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>101</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1255,11 +1323,14 @@
       <c r="G13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="16">
+        <v>200</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E14" s="4" t="s">
         <v>46</v>
       </c>
@@ -1269,11 +1340,14 @@
       <c r="G14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E15" s="4" t="s">
         <v>61</v>
       </c>
@@ -1283,11 +1357,14 @@
       <c r="G15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="16">
+        <v>204</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E16" s="4" t="s">
         <v>61</v>
       </c>
@@ -1297,11 +1374,14 @@
       <c r="G16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="16">
+        <v>204</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E17" s="4" t="s">
         <v>61</v>
       </c>
@@ -1311,11 +1391,14 @@
       <c r="G17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="16">
+        <v>204</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1325,11 +1408,14 @@
       <c r="G18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E19" s="4" t="s">
         <v>61</v>
       </c>
@@ -1339,11 +1425,14 @@
       <c r="G19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="16">
+        <v>204</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E20" s="4" t="s">
         <v>50</v>
       </c>
@@ -1353,11 +1442,14 @@
       <c r="G20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="16">
+        <v>204</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>50</v>
       </c>
@@ -1367,22 +1459,27 @@
       <c r="G21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="16">
+        <v>204</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="2:8" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="18" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="16"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E24" s="4" t="s">
         <v>19</v>
       </c>
@@ -1392,11 +1489,14 @@
       <c r="G24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="16">
+        <v>200</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
         <v>19</v>
       </c>
@@ -1406,22 +1506,27 @@
       <c r="G25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="16">
+        <v>200</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="2:8" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="18" t="s">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="16"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -1434,11 +1539,14 @@
       <c r="G28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="16">
+        <v>200</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E29" s="4" t="s">
         <v>61</v>
       </c>
@@ -1448,22 +1556,27 @@
       <c r="G29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="16">
+        <v>204</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="2:8" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="18" t="s">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="16"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E32" s="4" t="s">
         <v>19</v>
       </c>
@@ -1473,11 +1586,14 @@
       <c r="G32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="16">
+        <v>200</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E33" s="4" t="s">
         <v>46</v>
       </c>
@@ -1487,14 +1603,17 @@
       <c r="G33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="4">
+        <v>204</v>
+      </c>
+      <c r="I33" t="s">
         <v>45</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E34" s="4" t="s">
         <v>50</v>
       </c>
@@ -1504,11 +1623,14 @@
       <c r="G34" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="4">
+        <v>200</v>
+      </c>
+      <c r="I34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E35" s="4" t="s">
         <v>52</v>
       </c>
@@ -1518,19 +1640,23 @@
       <c r="G35" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="4">
+        <v>204</v>
+      </c>
+      <c r="I35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="2:9" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-      <c r="C37" s="18" t="s">
+    <row r="37" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E38" s="4" t="s">
         <v>19</v>
       </c>
@@ -1540,11 +1666,14 @@
       <c r="G38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="16">
+        <v>200</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E39" s="4" t="s">
         <v>19</v>
       </c>
@@ -1554,11 +1683,14 @@
       <c r="G39" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="16">
+        <v>200</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E40" s="4" t="s">
         <v>19</v>
       </c>
@@ -1568,11 +1700,14 @@
       <c r="G40" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="16">
+        <v>200</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E41" s="4" t="s">
         <v>19</v>
       </c>
@@ -1582,11 +1717,14 @@
       <c r="G41" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" s="16">
+        <v>200</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E42" s="4" t="s">
         <v>19</v>
       </c>
@@ -1596,11 +1734,14 @@
       <c r="G42" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" s="16">
+        <v>200</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E43" s="4" t="s">
         <v>19</v>
       </c>
@@ -1610,195 +1751,232 @@
       <c r="G43" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H43" s="16">
+        <v>200</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="2:9" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="C46" s="18" t="s">
+    <row r="45" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="8"/>
+      <c r="C45" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
+        <v>36</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="16">
+        <v>200</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E47" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="16">
+        <v>200</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H48" s="16"/>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="8"/>
+      <c r="C49" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="H49" s="13"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
         <v>36</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E48" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="G50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H50" s="16">
+        <v>200</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="2:8" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="9"/>
-      <c r="C50" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E51" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="G51" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="16">
+        <v>200</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="C53" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="H53" s="13"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
         <v>36</v>
       </c>
-      <c r="G51" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E52" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>24</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
-      <c r="C54" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E55" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="G54" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="16">
+        <v>200</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>36</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F56" t="s">
         <v>89</v>
       </c>
-      <c r="H56" s="3"/>
-    </row>
-    <row r="58" spans="2:8" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="9"/>
-      <c r="C58" s="18" t="s">
+      <c r="H55" s="16"/>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="57" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="8"/>
+      <c r="C57" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F59" t="s">
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="H57" s="13"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
         <v>90</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H58" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I58" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="2:8" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="9"/>
-      <c r="C61" s="18" t="s">
+    <row r="60" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="8"/>
+      <c r="C60" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="H60" s="13"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" t="s">
+        <v>92</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="16">
+        <v>200</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E62" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H62" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E63" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" t="s">
-        <v>93</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H63" s="3" t="s">
+      <c r="H62" s="16">
+        <v>200</v>
+      </c>
+      <c r="I62" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="2:9" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="9"/>
-      <c r="C65" s="18" t="s">
+    <row r="64" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="8"/>
+      <c r="C64" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H66" s="3" t="s">
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="H64" s="13"/>
+    </row>
+    <row r="65" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H65" s="16"/>
+      <c r="I65" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J65" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C49:E49"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reenabling support for composition with bundles
</commit_message>
<xml_diff>
--- a/MR3/tests/test odata stuff.xlsx
+++ b/MR3/tests/test odata stuff.xlsx
@@ -521,16 +521,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -540,9 +531,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,6 +539,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -901,7 +901,7 @@
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C27" sqref="C27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,69 +1112,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="G5" s="17" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="G5" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
@@ -1218,7 +1218,7 @@
       <c r="G7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="14">
         <v>200</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -1235,7 +1235,7 @@
       <c r="G8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="14">
         <v>200</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -1252,7 +1252,7 @@
       <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="14">
         <v>200</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -1269,7 +1269,7 @@
       <c r="G10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="14">
         <v>200</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -1286,7 +1286,7 @@
       <c r="G11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="14">
         <v>200</v>
       </c>
       <c r="I11" s="3" t="s">
@@ -1303,7 +1303,7 @@
       <c r="G12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="14">
         <v>200</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -1323,7 +1323,7 @@
       <c r="G13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="14">
         <v>200</v>
       </c>
       <c r="I13" s="3" t="s">
@@ -1340,7 +1340,7 @@
       <c r="G14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="14" t="s">
         <v>104</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -1357,7 +1357,7 @@
       <c r="G15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="14">
         <v>204</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -1374,7 +1374,7 @@
       <c r="G16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="14">
         <v>204</v>
       </c>
       <c r="I16" s="3" t="s">
@@ -1391,7 +1391,7 @@
       <c r="G17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="14">
         <v>204</v>
       </c>
       <c r="I17" s="3" t="s">
@@ -1408,7 +1408,7 @@
       <c r="G18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="14" t="s">
         <v>104</v>
       </c>
       <c r="I18" s="3" t="s">
@@ -1425,7 +1425,7 @@
       <c r="G19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="14">
         <v>204</v>
       </c>
       <c r="I19" s="3" t="s">
@@ -1442,7 +1442,7 @@
       <c r="G20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="14">
         <v>204</v>
       </c>
       <c r="I20" s="3" t="s">
@@ -1459,7 +1459,7 @@
       <c r="G21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="14">
         <v>204</v>
       </c>
       <c r="I21" s="3" t="s">
@@ -1467,16 +1467,16 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H22" s="16"/>
+      <c r="H22" s="14"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1489,7 +1489,7 @@
       <c r="G24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="14">
         <v>200</v>
       </c>
       <c r="I24" s="3" t="s">
@@ -1506,7 +1506,7 @@
       <c r="G25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="14">
         <v>200</v>
       </c>
       <c r="I25" s="3" t="s">
@@ -1514,16 +1514,16 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H26" s="16"/>
+      <c r="H26" s="14"/>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1539,7 +1539,7 @@
       <c r="G28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="14">
         <v>200</v>
       </c>
       <c r="I28" s="3" t="s">
@@ -1556,7 +1556,7 @@
       <c r="G29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="14">
         <v>204</v>
       </c>
       <c r="I29" s="3" t="s">
@@ -1564,16 +1564,16 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H30" s="16"/>
+      <c r="H30" s="14"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
       <c r="G32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="16">
+      <c r="H32" s="14">
         <v>200</v>
       </c>
       <c r="I32" s="3" t="s">
@@ -1649,11 +1649,11 @@
     </row>
     <row r="37" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -1666,7 +1666,7 @@
       <c r="G38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="16">
+      <c r="H38" s="14">
         <v>200</v>
       </c>
       <c r="I38" s="3" t="s">
@@ -1683,7 +1683,7 @@
       <c r="G39" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="16">
+      <c r="H39" s="14">
         <v>200</v>
       </c>
       <c r="I39" s="3" t="s">
@@ -1700,7 +1700,7 @@
       <c r="G40" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="16">
+      <c r="H40" s="14">
         <v>200</v>
       </c>
       <c r="I40" s="3" t="s">
@@ -1717,7 +1717,7 @@
       <c r="G41" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="16">
+      <c r="H41" s="14">
         <v>200</v>
       </c>
       <c r="I41" s="3" t="s">
@@ -1734,7 +1734,7 @@
       <c r="G42" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H42" s="16">
+      <c r="H42" s="14">
         <v>200</v>
       </c>
       <c r="I42" s="3" t="s">
@@ -1751,7 +1751,7 @@
       <c r="G43" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H43" s="16">
+      <c r="H43" s="14">
         <v>200</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -1760,11 +1760,11 @@
     </row>
     <row r="45" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -1777,7 +1777,7 @@
       <c r="G46" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H46" s="16">
+      <c r="H46" s="14">
         <v>200</v>
       </c>
       <c r="I46" s="3" t="s">
@@ -1794,7 +1794,7 @@
       <c r="G47" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H47" s="16">
+      <c r="H47" s="14">
         <v>200</v>
       </c>
       <c r="I47" s="3" t="s">
@@ -1802,16 +1802,16 @@
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H48" s="16"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="3"/>
     </row>
     <row r="49" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
       <c r="H49" s="13"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
       <c r="G50" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H50" s="16">
+      <c r="H50" s="14">
         <v>200</v>
       </c>
       <c r="I50" s="3" t="s">
@@ -1841,7 +1841,7 @@
       <c r="G51" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H51" s="16">
+      <c r="H51" s="14">
         <v>200</v>
       </c>
       <c r="I51" s="3" t="s">
@@ -1850,11 +1850,11 @@
     </row>
     <row r="53" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
       <c r="G54" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H54" s="16">
+      <c r="H54" s="14">
         <v>200</v>
       </c>
       <c r="I54" s="3" t="s">
@@ -1878,23 +1878,23 @@
       <c r="F55" t="s">
         <v>89</v>
       </c>
-      <c r="H55" s="16"/>
+      <c r="H55" s="14"/>
       <c r="I55" s="3"/>
     </row>
     <row r="57" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
         <v>90</v>
       </c>
-      <c r="H58" s="16" t="s">
+      <c r="H58" s="14" t="s">
         <v>103</v>
       </c>
       <c r="I58" s="3" t="s">
@@ -1903,11 +1903,11 @@
     </row>
     <row r="60" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
       <c r="G61" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H61" s="16">
+      <c r="H61" s="14">
         <v>200</v>
       </c>
       <c r="I61" s="3" t="s">
@@ -1937,7 +1937,7 @@
       <c r="G62" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H62" s="16">
+      <c r="H62" s="14">
         <v>200</v>
       </c>
       <c r="I62" s="3" t="s">
@@ -1946,15 +1946,15 @@
     </row>
     <row r="64" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H65" s="16"/>
+      <c r="H65" s="14"/>
       <c r="I65" s="3" t="s">
         <v>95</v>
       </c>
@@ -1964,12 +1964,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C45:E45"/>
@@ -1977,6 +1971,12 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated list of tests
</commit_message>
<xml_diff>
--- a/MR3/tests/test odata stuff.xlsx
+++ b/MR3/tests/test odata stuff.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="106">
   <si>
     <t>Missing features</t>
   </si>
@@ -540,11 +540,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,10 +1119,10 @@
         <v>35</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="21"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="18"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -1226,6 +1226,9 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1472,11 +1475,11 @@
     </row>
     <row r="23" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1519,11 +1522,11 @@
     </row>
     <row r="27" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1569,11 +1572,11 @@
     </row>
     <row r="31" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -1649,11 +1652,11 @@
     </row>
     <row r="37" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -1760,11 +1763,11 @@
     </row>
     <row r="45" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -1807,11 +1810,11 @@
     </row>
     <row r="49" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
       <c r="H49" s="13"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -1850,11 +1853,11 @@
     </row>
     <row r="53" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
@@ -1883,11 +1886,11 @@
     </row>
     <row r="57" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
@@ -1903,11 +1906,11 @@
     </row>
     <row r="60" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
@@ -1946,11 +1949,11 @@
     </row>
     <row r="64" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="8:10" x14ac:dyDescent="0.25">
@@ -1964,12 +1967,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C45:E45"/>
@@ -1977,6 +1974,12 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Support for serialization of primitives properties directlly
</commit_message>
<xml_diff>
--- a/MR3/tests/test odata stuff.xlsx
+++ b/MR3/tests/test odata stuff.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="106">
   <si>
     <t>Missing features</t>
   </si>
@@ -540,11 +540,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,10 +1119,10 @@
         <v>35</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="22"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="18"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -1246,6 +1246,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="E9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1475,11 +1478,11 @@
     </row>
     <row r="23" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1522,11 +1525,11 @@
     </row>
     <row r="27" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1572,11 +1575,11 @@
     </row>
     <row r="31" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -1652,11 +1655,11 @@
     </row>
     <row r="37" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -1763,11 +1766,11 @@
     </row>
     <row r="45" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -1810,11 +1813,11 @@
     </row>
     <row r="49" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
       <c r="H49" s="13"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -1853,11 +1856,11 @@
     </row>
     <row r="53" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
@@ -1886,11 +1889,11 @@
     </row>
     <row r="57" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
@@ -1906,11 +1909,11 @@
     </row>
     <row r="60" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
@@ -1949,11 +1952,11 @@
     </row>
     <row r="64" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="21" t="s">
+      <c r="C64" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="8:10" x14ac:dyDescent="0.25">
@@ -1967,6 +1970,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C45:E45"/>
@@ -1974,12 +1983,6 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Support for $value and fixes for resource id generation
</commit_message>
<xml_diff>
--- a/MR3/tests/test odata stuff.xlsx
+++ b/MR3/tests/test odata stuff.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="107">
   <si>
     <t>Missing features</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Op Result</t>
+  </si>
+  <si>
+    <t>plain</t>
   </si>
 </sst>
 </file>
@@ -540,11 +543,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1093,90 +1096,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="4" width="5.140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="43" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" customWidth="1"/>
+    <col min="2" max="5" width="5.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="43" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="15"/>
-    </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" s="6" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="19"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="19"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="15"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
       <c r="B3" s="20" t="s">
         <v>67</v>
       </c>
       <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="19"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="19"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="15"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="18"/>
       <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="20"/>
       <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="19"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="19"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="15"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="18"/>
       <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>97</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
-      <c r="G5" s="24" t="s">
+      <c r="E5" s="23"/>
+      <c r="H5" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
         <v>100</v>
       </c>
@@ -1186,803 +1194,822 @@
       <c r="D6" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="14">
-        <v>200</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="14">
+        <v>200</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="14">
-        <v>200</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="14">
+        <v>200</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="14">
-        <v>200</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="14">
+        <v>200</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="14">
-        <v>200</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="H10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="14">
+        <v>200</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="14">
-        <v>200</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="H11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="14">
+        <v>200</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="14">
-        <v>200</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="14">
+        <v>200</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="14">
-        <v>200</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="H13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="14">
+        <v>200</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E14" s="4" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="4" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="14">
+      <c r="I15" s="14">
         <v>204</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E16" s="4" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="14">
+      <c r="I16" s="14">
         <v>204</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="4" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="14">
+      <c r="I17" s="14">
         <v>204</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="I18" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E19" s="4" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="14">
+      <c r="I19" s="14">
         <v>204</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="s">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="14">
+      <c r="H20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="14">
         <v>204</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E21" s="4" t="s">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="14">
+      <c r="I21" s="14">
         <v>204</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H22" s="14"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="14"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="H23" s="13"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="14">
-        <v>200</v>
-      </c>
-      <c r="I24" s="3" t="s">
+      <c r="H24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="14">
+        <v>200</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" t="s">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="14">
-        <v>200</v>
-      </c>
-      <c r="I25" s="3" t="s">
+      <c r="H25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="14">
+        <v>200</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H26" s="14"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I26" s="14"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="H27" s="13"/>
-    </row>
-    <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="14">
-        <v>200</v>
-      </c>
-      <c r="I28" s="3" t="s">
+      <c r="H28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="14">
+        <v>200</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E29" s="4" t="s">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E29" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="14">
+      <c r="I29" s="14">
         <v>204</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H30" s="14"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I30" s="14"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="14">
-        <v>200</v>
-      </c>
-      <c r="I32" s="3" t="s">
+      <c r="H32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="14">
+        <v>200</v>
+      </c>
+      <c r="J32" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E33" s="4" t="s">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H33" s="4">
+      <c r="I33" s="4">
         <v>204</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>45</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E34" s="4" t="s">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F34" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="4">
-        <v>200</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="I34" s="4">
+        <v>200</v>
+      </c>
+      <c r="J34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E35" s="4" t="s">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H35" s="4">
+      <c r="I35" s="4">
         <v>204</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="H37" s="13"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" s="14">
-        <v>200</v>
-      </c>
-      <c r="I38" s="3" t="s">
+      <c r="H38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="14">
+        <v>200</v>
+      </c>
+      <c r="J38" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" t="s">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" s="14">
-        <v>200</v>
-      </c>
-      <c r="I39" s="3" t="s">
+      <c r="H39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="14">
+        <v>200</v>
+      </c>
+      <c r="J39" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" t="s">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" t="s">
         <v>74</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H40" s="14">
-        <v>200</v>
-      </c>
-      <c r="I40" s="3" t="s">
+      <c r="H40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="14">
+        <v>200</v>
+      </c>
+      <c r="J40" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" t="s">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" t="s">
         <v>75</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H41" s="14">
-        <v>200</v>
-      </c>
-      <c r="I41" s="3" t="s">
+      <c r="H41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="14">
+        <v>200</v>
+      </c>
+      <c r="J41" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E42" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" t="s">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" t="s">
         <v>77</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="14">
-        <v>200</v>
-      </c>
-      <c r="I42" s="3" t="s">
+      <c r="H42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="14">
+        <v>200</v>
+      </c>
+      <c r="J42" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H43" s="14">
-        <v>200</v>
-      </c>
-      <c r="I43" s="3" t="s">
+      <c r="H43" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" s="14">
+        <v>200</v>
+      </c>
+      <c r="J43" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="H45" s="13"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H46" s="14">
-        <v>200</v>
-      </c>
-      <c r="I46" s="3" t="s">
+      <c r="H46" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="14">
+        <v>200</v>
+      </c>
+      <c r="J46" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E47" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" t="s">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" t="s">
         <v>24</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H47" s="14">
-        <v>200</v>
-      </c>
-      <c r="I47" s="3" t="s">
+      <c r="H47" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="14">
+        <v>200</v>
+      </c>
+      <c r="J47" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H48" s="14"/>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I48" s="14"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="H49" s="13"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" t="s">
         <v>36</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H50" s="14">
-        <v>200</v>
-      </c>
-      <c r="I50" s="3" t="s">
+      <c r="H50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="14">
+        <v>200</v>
+      </c>
+      <c r="J50" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E51" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" t="s">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" t="s">
         <v>24</v>
       </c>
-      <c r="G51" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H51" s="14">
-        <v>200</v>
-      </c>
-      <c r="I51" s="3" t="s">
+      <c r="H51" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="14">
+        <v>200</v>
+      </c>
+      <c r="J51" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="H53" s="13"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E54" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" t="s">
         <v>36</v>
       </c>
-      <c r="G54" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="14">
-        <v>200</v>
-      </c>
-      <c r="I54" s="3" t="s">
+      <c r="H54" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" s="14">
+        <v>200</v>
+      </c>
+      <c r="J54" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F55" t="s">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
         <v>89</v>
       </c>
-      <c r="H55" s="14"/>
-      <c r="I55" s="3"/>
-    </row>
-    <row r="57" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="14"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="57" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="H57" s="13"/>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F58" t="s">
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
         <v>90</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="I58" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="I58" s="3" t="s">
+      <c r="J58" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="H60" s="13"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E61" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="I60" s="13"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" t="s">
         <v>92</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="14">
-        <v>200</v>
-      </c>
-      <c r="I61" s="3" t="s">
+      <c r="H61" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" s="14">
+        <v>200</v>
+      </c>
+      <c r="J61" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E62" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" t="s">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F62" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" t="s">
         <v>93</v>
       </c>
-      <c r="G62" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H62" s="14">
-        <v>200</v>
-      </c>
-      <c r="I62" s="3" t="s">
+      <c r="H62" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I62" s="14">
+        <v>200</v>
+      </c>
+      <c r="J62" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="2:9" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="H64" s="13"/>
-    </row>
-    <row r="65" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H65" s="14"/>
-      <c r="I65" s="3" t="s">
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="I64" s="13"/>
+    </row>
+    <row r="65" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I65" s="14"/>
+      <c r="J65" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J65" t="s">
+      <c r="K65" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Some refactoring to simplify code
</commit_message>
<xml_diff>
--- a/MR3/tests/test odata stuff.xlsx
+++ b/MR3/tests/test odata stuff.xlsx
@@ -1099,15 +1099,15 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="5" width="5.140625" style="9" customWidth="1"/>
+    <col min="2" max="5" width="4.140625" style="9" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" style="4" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="4" customWidth="1"/>
     <col min="10" max="10" width="43" customWidth="1"/>

</xml_diff>

<commit_message>
Added schema files and 3 failing tests for models with self relation
</commit_message>
<xml_diff>
--- a/MR3/tests/test odata stuff.xlsx
+++ b/MR3/tests/test odata stuff.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="107">
   <si>
     <t>Missing features</t>
   </si>
@@ -493,7 +493,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -543,17 +543,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1098,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1112,7 @@
     <col min="6" max="6" width="13.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="4" customWidth="1"/>
     <col min="10" max="10" width="43" customWidth="1"/>
     <col min="11" max="11" width="27.5703125" customWidth="1"/>
   </cols>
@@ -1123,10 +1126,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="15"/>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="18"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
@@ -1294,6 +1297,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1311,6 +1317,15 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F12" s="4" t="s">
         <v>19</v>
       </c>
@@ -1348,6 +1363,9 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F14" s="4" t="s">
         <v>46</v>
       </c>
@@ -1365,6 +1383,9 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F15" s="4" t="s">
         <v>61</v>
       </c>
@@ -1416,6 +1437,9 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1450,6 +1474,9 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F20" s="4" t="s">
         <v>50</v>
       </c>
@@ -1467,6 +1494,9 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="F21" s="4" t="s">
         <v>50</v>
       </c>
@@ -1489,12 +1519,12 @@
     </row>
     <row r="23" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1537,12 +1567,12 @@
     </row>
     <row r="27" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1594,12 +1624,12 @@
     </row>
     <row r="31" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1675,12 +1705,12 @@
     </row>
     <row r="37" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -1787,12 +1817,12 @@
     </row>
     <row r="45" spans="2:11" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -1835,12 +1865,12 @@
     </row>
     <row r="49" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -1879,12 +1909,12 @@
     </row>
     <row r="53" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -1913,12 +1943,12 @@
     </row>
     <row r="57" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -1934,12 +1964,12 @@
     </row>
     <row r="60" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
       <c r="I60" s="13"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -1978,12 +2008,12 @@
     </row>
     <row r="64" spans="2:10" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="21" t="s">
+      <c r="C64" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
       <c r="I64" s="13"/>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.25">
@@ -1997,6 +2027,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C45:F45"/>
@@ -2004,12 +2040,6 @@
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>